<commit_message>
creacion de la funcion de eliminar producto
</commit_message>
<xml_diff>
--- a/BaseCrudColabProductos.xlsx
+++ b/BaseCrudColabProductos.xlsx
@@ -425,29 +425,7 @@
         </is>
       </c>
     </row>
-    <row r="2">
-      <c r="A2" t="n">
-        <v>1</v>
-      </c>
-      <c r="B2" t="inlineStr">
-        <is>
-          <t>daniel</t>
-        </is>
-      </c>
-      <c r="C2" t="inlineStr">
-        <is>
-          <t>homo</t>
-        </is>
-      </c>
-      <c r="D2" t="n">
-        <v>0</v>
-      </c>
-      <c r="E2" t="inlineStr">
-        <is>
-          <t>10</t>
-        </is>
-      </c>
-    </row>
+    <row r="2"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
creacion de la funcion de actualizar producto
</commit_message>
<xml_diff>
--- a/BaseCrudColabProductos.xlsx
+++ b/BaseCrudColabProductos.xlsx
@@ -431,21 +431,19 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>daniel</t>
+          <t>yoiner</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>homo</t>
+          <t>gordo</t>
         </is>
       </c>
       <c r="D2" t="n">
-        <v>0</v>
-      </c>
-      <c r="E2" t="inlineStr">
-        <is>
-          <t>10</t>
-        </is>
+        <v>123</v>
+      </c>
+      <c r="E2" t="n">
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>